<commit_message>
Servo + Kurve Variante Hinzugefügt
</commit_message>
<xml_diff>
--- a/Nutzwertanalyse.xlsx
+++ b/Nutzwertanalyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98cd8e224f73c0f5/Desktop/newgit/komplexlab/Komplexlabor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{9CBBD041-98DE-4D39-BE51-DDB6F125F659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E94400E8-CDF5-4030-B6D9-7DBE1DFC9250}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{9CBBD041-98DE-4D39-BE51-DDB6F125F659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED09501-AF63-40AB-95B0-7090DC6C9689}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{D84C932A-B5BF-430A-B04A-EC047D0074B2}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Aufhängung" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Motor!$A$1:$O$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Motor!$A$1:$Q$19</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,16 +40,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
   <si>
     <t>Nutzwertanalyse</t>
   </si>
   <si>
     <t>Bewertungskriterien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variante 3
-</t>
   </si>
   <si>
     <t>Nr.</t>
@@ -148,6 +144,16 @@
   <si>
     <t>Variante 3
 Schrittmotor Seilzug</t>
+  </si>
+  <si>
+    <t>Variante 4
+Servo und Kurve</t>
+  </si>
+  <si>
+    <t>Eig</t>
+  </si>
+  <si>
+    <t>gew.Wert</t>
   </si>
 </sst>
 </file>
@@ -179,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -368,19 +374,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -612,11 +605,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -633,73 +681,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,13 +752,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1033,10 +1095,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="107" zoomScaleNormal="100" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="B1" zoomScale="107" zoomScaleNormal="100" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1053,10 +1115,11 @@
     <col min="11" max="11" width="5.54296875" customWidth="1"/>
     <col min="13" max="13" width="20.54296875" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5.54296875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" hidden="1" customWidth="1"/>
+    <col min="15" max="16" width="5.54296875" customWidth="1"/>
+    <col min="17" max="17" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -1073,111 +1136,123 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-    </row>
-    <row r="3" spans="1:15" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+    </row>
+    <row r="3" spans="1:17" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+        <v>24</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="25"/>
       <c r="J3" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="24"/>
       <c r="L3" s="25"/>
       <c r="M3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
         <v>2</v>
-      </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="39"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
-        <v>3</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="M4" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="O4" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="4">
         <v>5</v>
@@ -1187,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
@@ -1197,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="4">
         <v>0</v>
@@ -1208,33 +1283,39 @@
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="5">
-        <f t="shared" ref="O5:O18" si="1">C5*N5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="44">
+        <f>C5*P5</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F14" si="1">C6*E6</f>
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5">
-        <f t="shared" ref="F6:F14" si="2">C6*E6</f>
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H6" s="1">
         <v>10</v>
@@ -1244,128 +1325,146 @@
         <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1">
         <v>10</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" ref="L6:L16" si="3">C6*K6</f>
+        <f t="shared" ref="L6:L16" si="2">C6*K6</f>
         <v>50</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O6" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="44">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="44">
+        <f t="shared" ref="Q6:Q16" si="3">C6*P6</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" s="5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="1">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O7" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1">
-        <v>5</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="K8" s="1">
         <v>10</v>
       </c>
       <c r="L8" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O8" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="44">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="44">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
@@ -1375,7 +1474,7 @@
         <v>100</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1">
         <v>10</v>
@@ -1385,7 +1484,7 @@
         <v>200</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" s="1">
         <v>10</v>
@@ -1396,164 +1495,188 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="44">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="1">
-        <v>5</v>
-      </c>
-      <c r="I10" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="1">
-        <v>5</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O10" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="1">
-        <v>5</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O11" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="1">
-        <v>5</v>
-      </c>
-      <c r="I12" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="1">
-        <v>5</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O12" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>9</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1">
         <v>10</v>
@@ -1563,7 +1686,7 @@
         <v>100</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1">
         <v>10</v>
@@ -1573,7 +1696,7 @@
         <v>100</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K13" s="1">
         <v>5</v>
@@ -1584,70 +1707,82 @@
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O13" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="44">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3">
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1">
         <v>5</v>
       </c>
       <c r="F14" s="5">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="1">
-        <v>5</v>
-      </c>
-      <c r="I14" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="1">
-        <v>5</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O14" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="44">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3">
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1">
         <v>10</v>
@@ -1657,7 +1792,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="1">
         <v>5</v>
@@ -1667,34 +1802,40 @@
         <v>25</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O15" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="44">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="44">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3">
         <v>10</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1">
         <v>5</v>
@@ -1704,7 +1845,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -1714,23 +1855,29 @@
         <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K16" s="1">
         <v>10</v>
       </c>
       <c r="L16" s="5">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="M16" s="22"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="44">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="M16" s="22"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>13</v>
       </c>
@@ -1747,12 +1894,11 @@
       <c r="L17" s="5"/>
       <c r="M17" s="2"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12">
         <v>14</v>
       </c>
@@ -1764,27 +1910,26 @@
       <c r="G18" s="15"/>
       <c r="H18" s="13"/>
       <c r="I18" s="16"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="5"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="51"/>
       <c r="M18" s="15"/>
       <c r="N18" s="13"/>
-      <c r="O18" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+    </row>
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="17"/>
       <c r="B19" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="18">
         <f>SUM(C5:C18)</f>
         <v>100</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="18">
@@ -1792,7 +1937,7 @@
         <v>675</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18">
@@ -1800,41 +1945,41 @@
         <v>575</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K19" s="27"/>
-      <c r="L19" s="18">
+      <c r="L19" s="19">
         <f>SUM(L5:L18)</f>
         <v>700</v>
       </c>
-      <c r="M19" s="26" t="s">
-        <v>12</v>
+      <c r="M19" s="48" t="s">
+        <v>11</v>
       </c>
       <c r="N19" s="27"/>
-      <c r="O19" s="19">
-        <f>SUM(O5:O18)</f>
-        <v>0</v>
+      <c r="O19" s="52"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="19">
+        <f>SUM(Q5:Q18)</f>
+        <v>800</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="O19:P19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="15" max="1048575" man="1"/>
-  </colBreaks>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1876,60 +2021,60 @@
       <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="A2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="24"/>
-      <c r="F3" s="39"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="24"/>
-      <c r="I3" s="39"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2200,14 +2345,14 @@
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17"/>
       <c r="B19" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="18">
         <f>SUM(C5:C18)</f>
         <v>0</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="18">
@@ -2215,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18">
@@ -2268,73 +2413,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="A2" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="38"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2597,14 +2742,14 @@
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17"/>
       <c r="B19" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="18">
         <f>SUM(C5:C18)</f>
         <v>0</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="18">
@@ -2612,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18">

</xml_diff>